<commit_message>
Add hint with link to forum
</commit_message>
<xml_diff>
--- a/basic-forms/forms/app/dynamic_error_message.xlsx
+++ b/basic-forms/forms/app/dynamic_error_message.xlsx
@@ -83,13 +83,41 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">A hint that will be shown to the user below the question's label in smaller text.
+Can be translated.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">A hint that will be shown to the user below the question's label in smaller text.
+Can be translated.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">One or more modifiers that determine how the question will be displayed.
 These can be specific to the field type.</t>
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,21 +143,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">A message shown when the constraint expression evaluates to false.
 Can be translated.</t>
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -144,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -158,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -171,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -183,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -197,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -210,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -223,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -236,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -250,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -264,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -277,7 +304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -290,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="W1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -469,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -483,6 +510,12 @@
     <t xml:space="preserve">label::fr</t>
   </si>
   <si>
+    <t xml:space="preserve">hint::en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hint::fr</t>
+  </si>
+  <si>
     <t xml:space="preserve">appearance</t>
   </si>
   <si>
@@ -556,6 +589,39 @@
   </si>
   <si>
     <t xml:space="preserve">Entrez un nombre de 2 à 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See [this forum thread](https://forum.communityhealthtoolkit.org/t/how-to-list-multiple-constraint-messages-on-a-single-field-in-xlsform/960) for more context.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Voir [ce fil de discussion du forum](</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://forum.communityhealthtoolkit.org/t/how-to-list-multiple-constraint-messages-on-a-single-field-in-xlsform/960</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) pour plus de contexte.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">${my_num_issue} = ‘’</t>
@@ -649,7 +715,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -674,6 +740,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1124,14 +1197,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1140,23 +1213,24 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="30.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="53.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="22.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="21.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="21.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="19.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="24.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="27.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="23" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="30.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="53.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="22.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="21.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="21.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="19.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="24.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="27.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="25" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,22 +1246,22 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -1199,19 +1273,19 @@
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="3" t="s">
@@ -1222,129 +1296,139 @@
       </c>
       <c r="U1" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
-      <c r="U3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="W3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="H5" s="5"/>
-      <c r="I5" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="1"/>
+      <c r="K5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="N5" s="1"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
-      <c r="Q5" s="1"/>
+      <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="0"/>
-      <c r="XFB5" s="0"/>
-      <c r="XFC5" s="0"/>
-      <c r="XFD5" s="0"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
+      <c r="K6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
-      <c r="U6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="W6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1352,14 +1436,14 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I18:U9990 A17:B17 I17:U17 J7:U16 I11:I16 A18:G9990 E17:G17 A11:G16 A7:I9 A2:U2 A4:U4 H11:H9990">
+  <conditionalFormatting sqref="K18:W9990 A17:B17 K17:W17 L7:W16 K11:K16 G18:I9990 G17:I17 G11:I16 G7:K9 G2:W2 G4:W4 J11:J9990 A18:D9990 A11:D16 A7:D9 A2:D2 A4:D4 E2:F10000">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A2="begin_group"</formula>
     </cfRule>
@@ -1386,9 +1470,9 @@
       <formula>AND(ISBLANK(C2),NOT(OR(ISBLANK($A2),$A2="calculate")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11:I9990 I2 I7:I9 I4">
+  <conditionalFormatting sqref="K11:K9990 K2 K7:K9 K4">
     <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND($A2="calculate", ISBLANK(I2))</formula>
+      <formula>AND($A2="calculate", ISBLANK(K2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:D17">
@@ -1411,7 +1495,7 @@
       <formula>AND(ISBLANK(C17),NOT(OR(ISBLANK($A17),$A17="calculate")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:U3">
+  <conditionalFormatting sqref="G3:W3 A3:D3">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A3="begin_group"</formula>
     </cfRule>
@@ -1438,12 +1522,12 @@
       <formula>AND(ISBLANK(C3),NOT(OR(ISBLANK($A3),$A3="calculate")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
+  <conditionalFormatting sqref="K3">
     <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND($A3="calculate", ISBLANK(I3))</formula>
+      <formula>AND($A3="calculate", ISBLANK(K3))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:U6">
+  <conditionalFormatting sqref="G5:W6 A5:D6">
     <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A5="begin_group"</formula>
     </cfRule>
@@ -1470,9 +1554,9 @@
       <formula>AND(ISBLANK(C5),NOT(OR(ISBLANK($A5),$A5="calculate")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:I6">
+  <conditionalFormatting sqref="K5:K6">
     <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND($A5="calculate", ISBLANK(I5))</formula>
+      <formula>AND($A5="calculate", ISBLANK(K5))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
@@ -1484,15 +1568,18 @@
       <formula1>"begin_group,end_group,note,calculate,text,integer,decimal,select_one list_name,select_multiple list_name,date,time,datetime,begin_repeat,end_repeat,geopoint,geotrace,geoshape,start-geopoint,range,image,audio,video,file,rank,acknowledge,start,end,today"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L1005 Q2:Q1005 T2:T1005" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2:N1005 S2:S1005 V2:V1005" type="list">
       <formula1>"true"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S2:S1005" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U2:U1005" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId2" display="https://forum.communityhealthtoolkit.org/t/how-to-list-multiple-constraint-messages-on-a-single-field-in-xlsform/960"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1500,7 +1587,7 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1530,7 +1617,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1542,41 +1629,41 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1644,37 +1731,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C2" s="8" t="str">
         <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20250414135634</v>
+        <v>20250415081630</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>